<commit_message>
[FIX] zolib + z0bug_odoo
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/account_fiscal_year.xlsx
+++ b/z0bug_odoo/data/account_fiscal_year.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -37,6 +37,21 @@
     <t xml:space="preserve">status</t>
   </si>
   <si>
+    <t xml:space="preserve">z0bug.fy_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-12-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.fy_2020</t>
   </si>
   <si>
@@ -47,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">2020-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.fy_2021</t>
@@ -89,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,13 +191,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
   </cols>
@@ -254,6 +267,23 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>